<commit_message>
Bug fixment of  redirect
</commit_message>
<xml_diff>
--- a/tests/ExcelProcesser.Tests/resources/testData.xlsx
+++ b/tests/ExcelProcesser.Tests/resources/testData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23714"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428F561B-14C4-40F3-AA63-37FF01A7021A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FF6C4A-C023-4EE1-AF9B-F682C0AE30D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="140">
   <si>
     <t>Input</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -619,6 +619,51 @@
   </si>
   <si>
     <t>单码</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross area 4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cross_4A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cross_4B</t>
+  </si>
+  <si>
+    <t>Cross_4C</t>
+  </si>
+  <si>
+    <t>Cross_4D</t>
+  </si>
+  <si>
+    <t>Cross_4F</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cross_4G</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cross_4H</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cross_4J</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cross_4I</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cross_4K</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cross_4E</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1142,107 +1187,107 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="3" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="3" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="4">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="4" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="3" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="3" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="4">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="4" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="3" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="3" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1611,10 +1656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1937,7 +1982,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>0</v>
       </c>
@@ -1945,7 +1990,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" t="s">
         <v>120</v>
@@ -1957,7 +2002,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="C67" t="s">
         <v>122</v>
@@ -1966,71 +2011,95 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="33"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" t="s">
+        <v>130</v>
+      </c>
+      <c r="D72" t="s">
+        <v>133</v>
+      </c>
+      <c r="E72" t="s">
+        <v>134</v>
+      </c>
+      <c r="F72" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="C73" t="s">
+        <v>131</v>
+      </c>
+      <c r="D73" t="s">
+        <v>137</v>
+      </c>
+      <c r="E73" t="s">
+        <v>136</v>
+      </c>
+      <c r="F73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="C74" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="33"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="33"/>
+      <c r="C76" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="37" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B80" t="s">
         <v>52</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C80" t="s">
         <v>53</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D80" t="s">
         <v>54</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E80" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="37"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="37"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B79" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="37"/>
-      <c r="B80" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="37"/>
-      <c r="B81" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="37"/>
-      <c r="B82" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -2038,52 +2107,58 @@
         <v>0</v>
       </c>
       <c r="B87" t="s">
-        <v>44</v>
-      </c>
-      <c r="D87" t="s">
-        <v>45</v>
-      </c>
-      <c r="E87" t="s">
-        <v>46</v>
-      </c>
-      <c r="H87" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="37"/>
+      <c r="B88" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="37"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="37" t="s">
+      <c r="B89" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="37"/>
+      <c r="B90" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B93" t="s">
-        <v>78</v>
-      </c>
-      <c r="C93" t="s">
-        <v>79</v>
-      </c>
-      <c r="D93" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="37"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="37"/>
+      <c r="B95" t="s">
+        <v>44</v>
+      </c>
+      <c r="D95" t="s">
+        <v>45</v>
+      </c>
+      <c r="E95" t="s">
+        <v>46</v>
+      </c>
+      <c r="H95" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="37"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="37"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -2091,16 +2166,13 @@
         <v>0</v>
       </c>
       <c r="B101" t="s">
-        <v>61</v>
+        <v>78</v>
+      </c>
+      <c r="C101" t="s">
+        <v>79</v>
       </c>
       <c r="D101" t="s">
-        <v>62</v>
-      </c>
-      <c r="E101" t="s">
-        <v>63</v>
-      </c>
-      <c r="H101" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -2108,20 +2180,48 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="37"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" t="s">
+        <v>61</v>
+      </c>
+      <c r="D109" t="s">
+        <v>62</v>
+      </c>
+      <c r="E109" t="s">
+        <v>63</v>
+      </c>
+      <c r="H109" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="37"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A93:A95"/>
     <mergeCell ref="A101:A103"/>
+    <mergeCell ref="A109:A111"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="A87:A89"/>
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A95:A97"/>
     <mergeCell ref="A59:A61"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A32:A34"/>
@@ -2137,8 +2237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171B277E-1E9C-4949-8C4C-5EFD188DCF86}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2194,23 +2294,23 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="38"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="50"/>
       <c r="B3" s="3">
         <v>28</v>
       </c>
@@ -2235,7 +2335,7 @@
       <c r="I3" s="3">
         <v>35</v>
       </c>
-      <c r="J3" s="38"/>
+      <c r="J3" s="70"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2243,22 +2343,22 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="44"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="65"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="3">
         <v>28</v>
       </c>
@@ -2285,7 +2385,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="4">
         <v>1</v>
       </c>
@@ -2312,7 +2412,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="4">
         <v>1</v>
       </c>
@@ -2339,7 +2439,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="4">
@@ -2352,7 +2452,7 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
@@ -2365,7 +2465,7 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2378,7 +2478,7 @@
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2391,7 +2491,7 @@
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -2409,51 +2509,51 @@
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="48" t="s">
+      <c r="D23" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="41" t="s">
+      <c r="F23" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="I23" s="39" t="s">
+      <c r="I23" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="J23" s="41" t="s">
+      <c r="J23" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="K23" s="41" t="s">
+      <c r="K23" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L23" s="42"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="44"/>
-      <c r="T23" s="41" t="s">
+      <c r="L23" s="63"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="64"/>
+      <c r="P23" s="64"/>
+      <c r="Q23" s="64"/>
+      <c r="R23" s="64"/>
+      <c r="S23" s="65"/>
+      <c r="T23" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="U23" s="41" t="s">
+      <c r="U23" s="61" t="s">
         <v>91</v>
       </c>
       <c r="V23" s="53" t="s">
@@ -2468,31 +2568,31 @@
       <c r="Y23" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="Z23" s="50" t="s">
+      <c r="Z23" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="AA23" s="65" t="s">
+      <c r="AA23" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="AB23" s="65" t="s">
+      <c r="AB23" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="AC23" s="66" t="s">
+      <c r="AC23" s="39" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="62"/>
       <c r="L24" s="3">
         <v>28</v>
       </c>
@@ -2517,45 +2617,45 @@
       <c r="S24" s="3">
         <v>35</v>
       </c>
-      <c r="T24" s="40"/>
-      <c r="U24" s="40"/>
+      <c r="T24" s="62"/>
+      <c r="U24" s="62"/>
       <c r="V24" s="54"/>
       <c r="W24" s="56"/>
       <c r="X24" s="58"/>
       <c r="Y24" s="60"/>
-      <c r="Z24" s="50"/>
-      <c r="AA24" s="65"/>
-      <c r="AB24" s="65"/>
-      <c r="AC24" s="67"/>
+      <c r="Z24" s="46"/>
+      <c r="AA24" s="38"/>
+      <c r="AB24" s="38"/>
+      <c r="AC24" s="40"/>
     </row>
     <row r="25" spans="1:29" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
-      <c r="B25" s="64">
+      <c r="A25" s="50"/>
+      <c r="B25" s="41">
         <v>16501</v>
       </c>
-      <c r="C25" s="64">
+      <c r="C25" s="41">
         <v>91338035</v>
       </c>
       <c r="D25" s="7">
         <v>532325</v>
       </c>
-      <c r="E25" s="64" t="s">
+      <c r="E25" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="68" t="s">
+      <c r="F25" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="G25" s="64" t="s">
+      <c r="G25" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="H25" s="64"/>
-      <c r="I25" s="68" t="s">
+      <c r="H25" s="41"/>
+      <c r="I25" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="J25" s="68" t="s">
+      <c r="J25" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="K25" s="61" t="s">
+      <c r="K25" s="47" t="s">
         <v>126</v>
       </c>
       <c r="L25" s="4">
@@ -2595,13 +2695,13 @@
       <c r="W25" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="X25" s="69" t="s">
+      <c r="X25" s="43" t="s">
         <v>103</v>
       </c>
       <c r="Y25" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="Z25" s="70">
+      <c r="Z25" s="44">
         <v>43171</v>
       </c>
       <c r="AA25" s="12"/>
@@ -2612,19 +2712,19 @@
       </c>
     </row>
     <row r="26" spans="1:29" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
       <c r="D26" s="7">
         <v>532326</v>
       </c>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
-      <c r="K26" s="62"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="48"/>
       <c r="L26" s="4">
         <v>1</v>
       </c>
@@ -2662,11 +2762,11 @@
       <c r="W26" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="X26" s="69"/>
+      <c r="X26" s="43"/>
       <c r="Y26" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="Z26" s="71"/>
+      <c r="Z26" s="45"/>
       <c r="AA26" s="12"/>
       <c r="AB26" s="12"/>
       <c r="AC26" s="13">
@@ -2675,19 +2775,19 @@
       </c>
     </row>
     <row r="27" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="45"/>
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
       <c r="D27" s="7">
         <v>533180</v>
       </c>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="62" t="s">
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="48" t="s">
         <v>127</v>
       </c>
       <c r="L27" s="4"/>
@@ -2713,11 +2813,11 @@
       <c r="W27" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="X27" s="69"/>
+      <c r="X27" s="43"/>
       <c r="Y27" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="Z27" s="71"/>
+      <c r="Z27" s="45"/>
       <c r="AA27" s="12"/>
       <c r="AB27" s="12"/>
       <c r="AC27" s="13">
@@ -2726,19 +2826,19 @@
       </c>
     </row>
     <row r="28" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
       <c r="D28" s="7">
         <v>533181</v>
       </c>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64"/>
-      <c r="K28" s="62"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="48"/>
       <c r="L28" s="4"/>
       <c r="M28" s="5"/>
       <c r="N28" s="4"/>
@@ -2762,9 +2862,9 @@
       <c r="W28" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="X28" s="69"/>
+      <c r="X28" s="43"/>
       <c r="Y28" s="52"/>
-      <c r="Z28" s="71"/>
+      <c r="Z28" s="45"/>
       <c r="AA28" s="12"/>
       <c r="AB28" s="12"/>
       <c r="AC28" s="13">
@@ -2773,19 +2873,19 @@
       </c>
     </row>
     <row r="29" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A29" s="45"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="64"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
       <c r="D29" s="7">
         <v>533182</v>
       </c>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="62"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="48"/>
       <c r="L29" s="4"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
@@ -2809,9 +2909,9 @@
       <c r="W29" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="X29" s="69"/>
+      <c r="X29" s="43"/>
       <c r="Y29" s="52"/>
-      <c r="Z29" s="50"/>
+      <c r="Z29" s="46"/>
       <c r="AA29" s="12"/>
       <c r="AB29" s="12"/>
       <c r="AC29" s="13">
@@ -2820,19 +2920,19 @@
       </c>
     </row>
     <row r="30" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="64"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
       <c r="D30" s="7">
         <v>533183</v>
       </c>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="62"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="48"/>
       <c r="L30" s="4"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
@@ -2856,9 +2956,9 @@
       <c r="W30" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="X30" s="69"/>
+      <c r="X30" s="43"/>
       <c r="Y30" s="52"/>
-      <c r="Z30" s="50"/>
+      <c r="Z30" s="46"/>
       <c r="AA30" s="12"/>
       <c r="AB30" s="12"/>
       <c r="AC30" s="13">
@@ -2867,19 +2967,19 @@
       </c>
     </row>
     <row r="31" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="45"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="64"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
       <c r="D31" s="7">
         <v>533184</v>
       </c>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="64"/>
-      <c r="K31" s="63"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="49"/>
       <c r="L31" s="4"/>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
@@ -2903,9 +3003,9 @@
       <c r="W31" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="X31" s="69"/>
+      <c r="X31" s="43"/>
       <c r="Y31" s="52"/>
-      <c r="Z31" s="50"/>
+      <c r="Z31" s="46"/>
       <c r="AA31" s="12"/>
       <c r="AB31" s="12"/>
       <c r="AC31" s="13">
@@ -2914,26 +3014,26 @@
       </c>
     </row>
     <row r="32" spans="1:29" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A32" s="45"/>
-      <c r="B32" s="64"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="64"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="64"/>
-      <c r="O32" s="64"/>
-      <c r="P32" s="64"/>
-      <c r="Q32" s="64"/>
-      <c r="R32" s="64"/>
-      <c r="S32" s="64"/>
-      <c r="T32" s="64"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="41"/>
+      <c r="R32" s="41"/>
+      <c r="S32" s="41"/>
+      <c r="T32" s="41"/>
       <c r="U32" s="15">
         <f>SUM(U25:U31)</f>
         <v>298</v>
@@ -2960,7 +3060,7 @@
       </c>
     </row>
     <row r="33" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A33" s="45"/>
+      <c r="A33" s="50"/>
       <c r="B33" s="20" t="s">
         <v>109</v>
       </c>
@@ -3002,6 +3102,33 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="B32:T32"/>
+    <mergeCell ref="A23:A33"/>
+    <mergeCell ref="AA23:AA24"/>
+    <mergeCell ref="Y27:Y31"/>
+    <mergeCell ref="V23:V24"/>
+    <mergeCell ref="W23:W24"/>
+    <mergeCell ref="X23:X24"/>
+    <mergeCell ref="Y23:Y24"/>
+    <mergeCell ref="Z23:Z24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="L23:S23"/>
+    <mergeCell ref="T23:T24"/>
+    <mergeCell ref="U23:U24"/>
     <mergeCell ref="AB23:AB24"/>
     <mergeCell ref="AC23:AC24"/>
     <mergeCell ref="B25:B31"/>
@@ -3016,33 +3143,6 @@
     <mergeCell ref="Z25:Z31"/>
     <mergeCell ref="K25:K26"/>
     <mergeCell ref="K27:K31"/>
-    <mergeCell ref="B32:T32"/>
-    <mergeCell ref="A23:A33"/>
-    <mergeCell ref="AA23:AA24"/>
-    <mergeCell ref="Y27:Y31"/>
-    <mergeCell ref="V23:V24"/>
-    <mergeCell ref="W23:W24"/>
-    <mergeCell ref="X23:X24"/>
-    <mergeCell ref="Y23:Y24"/>
-    <mergeCell ref="Z23:Z24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="L23:S23"/>
-    <mergeCell ref="T23:T24"/>
-    <mergeCell ref="U23:U24"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Try add logger in stream
</commit_message>
<xml_diff>
--- a/tests/ExcelProcesser.Tests/resources/testData.xlsx
+++ b/tests/ExcelProcesser.Tests/resources/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23714"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FF6C4A-C023-4EE1-AF9B-F682C0AE30D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86C72F6-FED4-4F5C-882C-A8AD4B19DD62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1187,16 +1187,85 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="3" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="4">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="4" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="3" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="3" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1211,9 +1280,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1221,72 +1287,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="4">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="4" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="3" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1658,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2294,23 +2294,23 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="70"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="3">
         <v>28</v>
       </c>
@@ -2335,7 +2335,7 @@
       <c r="I3" s="3">
         <v>35</v>
       </c>
-      <c r="J3" s="70"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2343,22 +2343,22 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="65"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="44"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="3">
         <v>28</v>
       </c>
@@ -2385,7 +2385,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="4">
         <v>1</v>
       </c>
@@ -2412,7 +2412,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="4">
         <v>1</v>
       </c>
@@ -2439,7 +2439,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="4">
@@ -2452,7 +2452,7 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
@@ -2465,7 +2465,7 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2478,7 +2478,7 @@
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
+      <c r="A15" s="45"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2491,7 +2491,7 @@
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -2509,90 +2509,90 @@
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="68" t="s">
+      <c r="D23" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="61" t="s">
+      <c r="E23" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="61" t="s">
+      <c r="F23" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="G23" s="71" t="s">
+      <c r="G23" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="61" t="s">
+      <c r="H23" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="I23" s="71" t="s">
+      <c r="I23" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="J23" s="61" t="s">
+      <c r="J23" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="K23" s="61" t="s">
+      <c r="K23" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="L23" s="63"/>
-      <c r="M23" s="64"/>
-      <c r="N23" s="64"/>
-      <c r="O23" s="64"/>
-      <c r="P23" s="64"/>
-      <c r="Q23" s="64"/>
-      <c r="R23" s="64"/>
-      <c r="S23" s="65"/>
-      <c r="T23" s="61" t="s">
+      <c r="L23" s="42"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="43"/>
+      <c r="S23" s="44"/>
+      <c r="T23" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="U23" s="61" t="s">
+      <c r="U23" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="V23" s="53" t="s">
+      <c r="V23" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="W23" s="55" t="s">
+      <c r="W23" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="X23" s="57" t="s">
+      <c r="X23" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="Y23" s="59" t="s">
+      <c r="Y23" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="Z23" s="46" t="s">
+      <c r="Z23" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="AA23" s="38" t="s">
+      <c r="AA23" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="AB23" s="38" t="s">
+      <c r="AB23" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="AC23" s="39" t="s">
+      <c r="AC23" s="63" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="62"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
       <c r="L24" s="3">
         <v>28</v>
       </c>
@@ -2617,45 +2617,45 @@
       <c r="S24" s="3">
         <v>35</v>
       </c>
-      <c r="T24" s="62"/>
-      <c r="U24" s="62"/>
-      <c r="V24" s="54"/>
-      <c r="W24" s="56"/>
-      <c r="X24" s="58"/>
-      <c r="Y24" s="60"/>
-      <c r="Z24" s="46"/>
-      <c r="AA24" s="38"/>
-      <c r="AB24" s="38"/>
-      <c r="AC24" s="40"/>
+      <c r="T24" s="40"/>
+      <c r="U24" s="40"/>
+      <c r="V24" s="55"/>
+      <c r="W24" s="57"/>
+      <c r="X24" s="59"/>
+      <c r="Y24" s="61"/>
+      <c r="Z24" s="62"/>
+      <c r="AA24" s="51"/>
+      <c r="AB24" s="51"/>
+      <c r="AC24" s="64"/>
     </row>
     <row r="25" spans="1:29" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="41">
+      <c r="A25" s="45"/>
+      <c r="B25" s="50">
         <v>16501</v>
       </c>
-      <c r="C25" s="41">
+      <c r="C25" s="50">
         <v>91338035</v>
       </c>
       <c r="D25" s="7">
         <v>532325</v>
       </c>
-      <c r="E25" s="41" t="s">
+      <c r="E25" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="42" t="s">
+      <c r="F25" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="G25" s="41" t="s">
+      <c r="G25" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="H25" s="41"/>
-      <c r="I25" s="42" t="s">
+      <c r="H25" s="50"/>
+      <c r="I25" s="65" t="s">
         <v>100</v>
       </c>
-      <c r="J25" s="42" t="s">
+      <c r="J25" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="K25" s="47" t="s">
+      <c r="K25" s="69" t="s">
         <v>126</v>
       </c>
       <c r="L25" s="4">
@@ -2695,13 +2695,13 @@
       <c r="W25" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="X25" s="43" t="s">
+      <c r="X25" s="66" t="s">
         <v>103</v>
       </c>
       <c r="Y25" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="Z25" s="44">
+      <c r="Z25" s="67">
         <v>43171</v>
       </c>
       <c r="AA25" s="12"/>
@@ -2712,19 +2712,19 @@
       </c>
     </row>
     <row r="26" spans="1:29" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="7">
         <v>532326</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="48"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="70"/>
       <c r="L26" s="4">
         <v>1</v>
       </c>
@@ -2762,11 +2762,11 @@
       <c r="W26" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="X26" s="43"/>
+      <c r="X26" s="66"/>
       <c r="Y26" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="Z26" s="45"/>
+      <c r="Z26" s="68"/>
       <c r="AA26" s="12"/>
       <c r="AB26" s="12"/>
       <c r="AC26" s="13">
@@ -2775,19 +2775,19 @@
       </c>
     </row>
     <row r="27" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="7">
         <v>533180</v>
       </c>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="48" t="s">
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="70" t="s">
         <v>127</v>
       </c>
       <c r="L27" s="4"/>
@@ -2813,11 +2813,11 @@
       <c r="W27" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="X27" s="43"/>
-      <c r="Y27" s="51" t="s">
+      <c r="X27" s="66"/>
+      <c r="Y27" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="Z27" s="45"/>
+      <c r="Z27" s="68"/>
       <c r="AA27" s="12"/>
       <c r="AB27" s="12"/>
       <c r="AC27" s="13">
@@ -2826,19 +2826,19 @@
       </c>
     </row>
     <row r="28" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="7">
         <v>533181</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="48"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="70"/>
       <c r="L28" s="4"/>
       <c r="M28" s="5"/>
       <c r="N28" s="4"/>
@@ -2862,9 +2862,9 @@
       <c r="W28" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="X28" s="43"/>
-      <c r="Y28" s="52"/>
-      <c r="Z28" s="45"/>
+      <c r="X28" s="66"/>
+      <c r="Y28" s="53"/>
+      <c r="Z28" s="68"/>
       <c r="AA28" s="12"/>
       <c r="AB28" s="12"/>
       <c r="AC28" s="13">
@@ -2873,19 +2873,19 @@
       </c>
     </row>
     <row r="29" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
       <c r="D29" s="7">
         <v>533182</v>
       </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="48"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="70"/>
       <c r="L29" s="4"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
@@ -2909,9 +2909,9 @@
       <c r="W29" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="X29" s="43"/>
-      <c r="Y29" s="52"/>
-      <c r="Z29" s="46"/>
+      <c r="X29" s="66"/>
+      <c r="Y29" s="53"/>
+      <c r="Z29" s="62"/>
       <c r="AA29" s="12"/>
       <c r="AB29" s="12"/>
       <c r="AC29" s="13">
@@ -2920,19 +2920,19 @@
       </c>
     </row>
     <row r="30" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
+      <c r="A30" s="45"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="7">
         <v>533183</v>
       </c>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="48"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="70"/>
       <c r="L30" s="4"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
@@ -2956,9 +2956,9 @@
       <c r="W30" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="X30" s="43"/>
-      <c r="Y30" s="52"/>
-      <c r="Z30" s="46"/>
+      <c r="X30" s="66"/>
+      <c r="Y30" s="53"/>
+      <c r="Z30" s="62"/>
       <c r="AA30" s="12"/>
       <c r="AB30" s="12"/>
       <c r="AC30" s="13">
@@ -2967,19 +2967,19 @@
       </c>
     </row>
     <row r="31" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
+      <c r="A31" s="45"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
       <c r="D31" s="7">
         <v>533184</v>
       </c>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="49"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="71"/>
       <c r="L31" s="4"/>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
@@ -3003,9 +3003,9 @@
       <c r="W31" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="X31" s="43"/>
-      <c r="Y31" s="52"/>
-      <c r="Z31" s="46"/>
+      <c r="X31" s="66"/>
+      <c r="Y31" s="53"/>
+      <c r="Z31" s="62"/>
       <c r="AA31" s="12"/>
       <c r="AB31" s="12"/>
       <c r="AC31" s="13">
@@ -3014,26 +3014,26 @@
       </c>
     </row>
     <row r="32" spans="1:29" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="41"/>
-      <c r="M32" s="41"/>
-      <c r="N32" s="41"/>
-      <c r="O32" s="41"/>
-      <c r="P32" s="41"/>
-      <c r="Q32" s="41"/>
-      <c r="R32" s="41"/>
-      <c r="S32" s="41"/>
-      <c r="T32" s="41"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="50"/>
+      <c r="L32" s="50"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="50"/>
+      <c r="P32" s="50"/>
+      <c r="Q32" s="50"/>
+      <c r="R32" s="50"/>
+      <c r="S32" s="50"/>
+      <c r="T32" s="50"/>
       <c r="U32" s="15">
         <f>SUM(U25:U31)</f>
         <v>298</v>
@@ -3060,7 +3060,7 @@
       </c>
     </row>
     <row r="33" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
+      <c r="A33" s="45"/>
       <c r="B33" s="20" t="s">
         <v>109</v>
       </c>
@@ -3102,19 +3102,20 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="AB23:AB24"/>
+    <mergeCell ref="AC23:AC24"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="E25:E31"/>
+    <mergeCell ref="F25:F31"/>
+    <mergeCell ref="G25:G31"/>
+    <mergeCell ref="H25:H31"/>
+    <mergeCell ref="I25:I31"/>
+    <mergeCell ref="J25:J31"/>
+    <mergeCell ref="X25:X31"/>
+    <mergeCell ref="Z25:Z31"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="K27:K31"/>
     <mergeCell ref="B32:T32"/>
     <mergeCell ref="A23:A33"/>
     <mergeCell ref="AA23:AA24"/>
@@ -3129,20 +3130,19 @@
     <mergeCell ref="L23:S23"/>
     <mergeCell ref="T23:T24"/>
     <mergeCell ref="U23:U24"/>
-    <mergeCell ref="AB23:AB24"/>
-    <mergeCell ref="AC23:AC24"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="C25:C31"/>
-    <mergeCell ref="E25:E31"/>
-    <mergeCell ref="F25:F31"/>
-    <mergeCell ref="G25:G31"/>
-    <mergeCell ref="H25:H31"/>
-    <mergeCell ref="I25:I31"/>
-    <mergeCell ref="J25:J31"/>
-    <mergeCell ref="X25:X31"/>
-    <mergeCell ref="Z25:Z31"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="K27:K31"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>